<commit_message>
final changes, comments deleted, unused code deleted
</commit_message>
<xml_diff>
--- a/Dane do pracy magisterskiej.xlsx
+++ b/Dane do pracy magisterskiej.xlsx
@@ -9,13 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17235" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17235" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
     <sheet name="Arkusz2" sheetId="2" r:id="rId2"/>
     <sheet name="Arkusz3" sheetId="3" r:id="rId3"/>
-    <sheet name="Arkusz4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -218,13 +217,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -514,16 +513,16 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="J1" s="1" t="s">
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="J1" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
     </row>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D2">
@@ -546,7 +545,7 @@
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C3">
@@ -561,7 +560,7 @@
       <c r="F3" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="I3">
@@ -578,7 +577,7 @@
       </c>
     </row>
     <row r="4" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
+      <c r="B4" s="5"/>
       <c r="C4" t="s">
         <v>9</v>
       </c>
@@ -591,7 +590,7 @@
       <c r="F4" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="1"/>
+      <c r="H4" s="5"/>
       <c r="I4" t="s">
         <v>9</v>
       </c>
@@ -606,7 +605,7 @@
       </c>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="1"/>
+      <c r="B5" s="5"/>
       <c r="C5" t="s">
         <v>10</v>
       </c>
@@ -619,7 +618,7 @@
       <c r="F5" t="s">
         <v>8</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="5"/>
       <c r="I5" t="s">
         <v>10</v>
       </c>
@@ -634,11 +633,11 @@
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D9" s="1" t="s">
+      <c r="D9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D10">
@@ -652,7 +651,7 @@
       </c>
     </row>
     <row r="11" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C11">
@@ -669,7 +668,7 @@
       </c>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="1"/>
+      <c r="B12" s="5"/>
       <c r="C12" t="s">
         <v>9</v>
       </c>
@@ -684,7 +683,7 @@
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B13" s="1"/>
+      <c r="B13" s="5"/>
       <c r="C13" t="s">
         <v>10</v>
       </c>
@@ -699,11 +698,11 @@
       </c>
     </row>
     <row r="17" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
     </row>
     <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="D18">
@@ -717,34 +716,34 @@
       </c>
     </row>
     <row r="19" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>1</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E19" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="2" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="20" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B20" s="1"/>
+      <c r="B20" s="5"/>
       <c r="C20" t="s">
         <v>9</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="2" t="s">
         <v>25</v>
       </c>
       <c r="O20" t="s">
@@ -758,17 +757,17 @@
       </c>
     </row>
     <row r="21" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B21" s="1"/>
+      <c r="B21" s="5"/>
       <c r="C21" t="s">
         <v>10</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="3" t="s">
+      <c r="E21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="2" t="s">
         <v>27</v>
       </c>
       <c r="O21" t="s">
@@ -802,15 +801,15 @@
       <c r="Q29">
         <v>26.79</v>
       </c>
-      <c r="S29" s="3">
+      <c r="S29" s="2">
         <f>ROUND($O$29/O29,4)</f>
         <v>1</v>
       </c>
-      <c r="T29" s="3">
+      <c r="T29" s="2">
         <f t="shared" ref="T29:U29" si="0">ROUND($O$29/P29,4)</f>
         <v>1.8230999999999999</v>
       </c>
-      <c r="U29" s="3">
+      <c r="U29" s="2">
         <f t="shared" si="0"/>
         <v>2.8656000000000001</v>
       </c>
@@ -822,18 +821,18 @@
       <c r="P30">
         <v>37.33</v>
       </c>
-      <c r="Q30" s="2">
+      <c r="Q30" s="1">
         <v>25.3</v>
       </c>
-      <c r="S30" s="3">
+      <c r="S30" s="2">
         <f t="shared" ref="S30:S31" si="1">ROUND($O$29/O30,4)</f>
         <v>1.1627000000000001</v>
       </c>
-      <c r="T30" s="3">
+      <c r="T30" s="2">
         <f t="shared" ref="T30:T31" si="2">ROUND($O$29/P30,4)</f>
         <v>2.0565000000000002</v>
       </c>
-      <c r="U30" s="3">
+      <c r="U30" s="2">
         <f t="shared" ref="U30:U31" si="3">ROUND($O$29/Q30,4)</f>
         <v>3.0344000000000002</v>
       </c>
@@ -848,15 +847,15 @@
       <c r="Q31">
         <v>23.58</v>
       </c>
-      <c r="S31" s="3">
+      <c r="S31" s="2">
         <f t="shared" si="1"/>
         <v>1.3223</v>
       </c>
-      <c r="T31" s="3">
+      <c r="T31" s="2">
         <f t="shared" si="2"/>
         <v>2.3109999999999999</v>
       </c>
-      <c r="U31" s="3">
+      <c r="U31" s="2">
         <f t="shared" si="3"/>
         <v>3.2557</v>
       </c>
@@ -1815,13 +1814,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M10" sqref="I1:M10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="7" max="7" width="9.140625" style="4"/>
+    <col min="7" max="7" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.25">
@@ -1840,27 +1839,27 @@
       <c r="E1">
         <v>30.8</v>
       </c>
-      <c r="G1" s="5"/>
-      <c r="I1" s="2">
+      <c r="G1" s="4"/>
+      <c r="I1" s="1">
         <v>9.75</v>
       </c>
-      <c r="J1" s="2">
+      <c r="J1" s="1">
         <v>9.8699999999999992</v>
       </c>
-      <c r="K1" s="2">
+      <c r="K1" s="1">
         <v>10.130000000000001</v>
       </c>
-      <c r="L1" s="2">
+      <c r="L1" s="1">
         <v>10.199999999999999</v>
       </c>
-      <c r="M1" s="2">
+      <c r="M1" s="1">
         <v>9.91</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -1878,27 +1877,27 @@
       <c r="E2">
         <v>30.81</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="4"/>
       <c r="I2">
         <v>9.75</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="1">
         <v>9.6300000000000008</v>
       </c>
-      <c r="K2" s="2">
+      <c r="K2" s="1">
         <v>9.92</v>
       </c>
-      <c r="L2" s="2">
+      <c r="L2" s="1">
         <v>10.01</v>
       </c>
-      <c r="M2" s="2">
+      <c r="M2" s="1">
         <v>9.74</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1916,7 +1915,7 @@
       <c r="E3">
         <v>30.58</v>
       </c>
-      <c r="G3" s="5"/>
+      <c r="G3" s="4"/>
       <c r="I3">
         <v>9.69</v>
       </c>
@@ -1949,7 +1948,7 @@
       <c r="E4">
         <v>30.59</v>
       </c>
-      <c r="G4" s="5"/>
+      <c r="G4" s="4"/>
       <c r="I4">
         <v>9.7200000000000006</v>
       </c>
@@ -1982,7 +1981,7 @@
       <c r="E5">
         <v>31.22</v>
       </c>
-      <c r="G5" s="5"/>
+      <c r="G5" s="4"/>
       <c r="I5">
         <v>9.7799999999999994</v>
       </c>
@@ -2015,7 +2014,7 @@
       <c r="E6">
         <v>29.67</v>
       </c>
-      <c r="G6" s="5"/>
+      <c r="G6" s="4"/>
       <c r="I6">
         <v>9.77</v>
       </c>
@@ -2048,7 +2047,7 @@
       <c r="E7">
         <v>29.74</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="4"/>
       <c r="I7">
         <v>10.32</v>
       </c>
@@ -2081,7 +2080,7 @@
       <c r="E8">
         <v>30.99</v>
       </c>
-      <c r="G8" s="5"/>
+      <c r="G8" s="4"/>
       <c r="I8">
         <v>9.86</v>
       </c>
@@ -2114,7 +2113,7 @@
       <c r="E9">
         <v>30.38</v>
       </c>
-      <c r="G9" s="5"/>
+      <c r="G9" s="4"/>
       <c r="I9">
         <v>9.7799999999999994</v>
       </c>
@@ -2147,7 +2146,7 @@
       <c r="E10">
         <v>30.56</v>
       </c>
-      <c r="G10" s="5"/>
+      <c r="G10" s="4"/>
       <c r="I10">
         <v>10.36</v>
       </c>
@@ -2165,62 +2164,48 @@
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G11" s="5"/>
+      <c r="G11" s="4"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G12" s="5"/>
+      <c r="G12" s="4"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G13" s="5"/>
+      <c r="G13" s="4"/>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G14" s="5"/>
+      <c r="G14" s="4"/>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G15" s="5"/>
+      <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="G16" s="5"/>
+      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17" s="5"/>
+      <c r="G17" s="4"/>
     </row>
     <row r="18" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G18" s="5"/>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G19" s="5"/>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G20" s="5"/>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G21" s="5"/>
+      <c r="G21" s="4"/>
     </row>
     <row r="22" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G22" s="5"/>
+      <c r="G22" s="4"/>
     </row>
     <row r="23" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G23" s="5"/>
+      <c r="G23" s="4"/>
     </row>
     <row r="24" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G24" s="5"/>
+      <c r="G24" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>